<commit_message>
added:add functionality of lagout
</commit_message>
<xml_diff>
--- a/build/resources/test/FBTestFile1.xlsx
+++ b/build/resources/test/FBTestFile1.xlsx
@@ -136,7 +136,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -148,7 +148,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -157,7 +157,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="sweetpinu@93"/>
+    <hyperlink ref="A1" r:id="rId1" display="khairnarswapna93@gmail.com"/>
+    <hyperlink ref="B1" r:id="rId2" display="sweetpinu@93"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>